<commit_message>
Added Spotlight with Street lamp
</commit_message>
<xml_diff>
--- a/CG Lab Project Submission Checklist.xlsx
+++ b/CG Lab Project Submission Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="58">
   <si>
     <t>Project Name:</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Ice sculpture</t>
+  </si>
+  <si>
+    <t>Street Lamp</t>
+  </si>
+  <si>
+    <t>Ice / Beach / Forest</t>
   </si>
 </sst>
 </file>
@@ -576,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -911,8 +917,12 @@
       <c r="A11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
@@ -1618,7 +1628,9 @@
       <c r="B33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="3"/>
+      <c r="C33" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
@@ -1681,7 +1693,9 @@
       <c r="A35" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="3"/>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="C35" s="3" t="s">
         <v>50</v>
       </c>
@@ -1870,9 +1884,11 @@
         <v>44</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
-      <c r="C41" s="3"/>
+      <c r="C41" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
       <c r="F41" s="3"/>

</xml_diff>

<commit_message>
Made camera time dependent
</commit_message>
<xml_diff>
--- a/CG Lab Project Submission Checklist.xlsx
+++ b/CG Lab Project Submission Checklist.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
   <si>
     <t>Project Name:</t>
   </si>
@@ -27,13 +27,7 @@
     <t>Student 1 (+workload):</t>
   </si>
   <si>
-    <t>WORKLOAD%_STUD1</t>
-  </si>
-  <si>
     <t>Student 2 (+workload):</t>
-  </si>
-  <si>
-    <t>WORKLOAD%_STUD2</t>
   </si>
   <si>
     <t>(see CG Lab Specification SS2017 for details)</t>
@@ -168,9 +162,6 @@
     <t>Most of the nodes</t>
   </si>
   <si>
-    <t>Billboarding Texture</t>
-  </si>
-  <si>
     <t>Sun/Moon</t>
   </si>
   <si>
@@ -178,12 +169,6 @@
   </si>
   <si>
     <t>Done per water shader</t>
-  </si>
-  <si>
-    <t>Snowman</t>
-  </si>
-  <si>
-    <t>Ice sculpture</t>
   </si>
   <si>
     <t>Street Lamp</t>
@@ -194,12 +179,24 @@
   <si>
     <t>Multiple Characters</t>
   </si>
+  <si>
+    <t>Snowman / Dragon</t>
+  </si>
+  <si>
+    <t>Ice sculpture / Pool Edge / Car Front / Car Back</t>
+  </si>
+  <si>
+    <t>Billboarding / Fence / Floor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -226,6 +223,11 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -250,10 +252,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -266,8 +269,11 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -582,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
@@ -598,7 +604,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
@@ -629,11 +635,11 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>1555054</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
+      <c r="C2" s="9">
+        <v>0.6</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -661,13 +667,13 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2">
         <v>855805</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>4</v>
+      <c r="C3" s="9">
+        <v>0.4</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -695,7 +701,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
@@ -753,13 +759,13 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
@@ -787,7 +793,7 @@
     </row>
     <row r="7" spans="1:26">
       <c r="A7" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -817,10 +823,10 @@
     </row>
     <row r="8" spans="1:26">
       <c r="A8" s="6" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -849,13 +855,13 @@
     </row>
     <row r="9" spans="1:26">
       <c r="A9" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -883,13 +889,13 @@
     </row>
     <row r="10" spans="1:26">
       <c r="A10" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
@@ -917,13 +923,13 @@
     </row>
     <row r="11" spans="1:26">
       <c r="A11" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -951,10 +957,10 @@
     </row>
     <row r="12" spans="1:26">
       <c r="A12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -983,13 +989,13 @@
     </row>
     <row r="13" spans="1:26">
       <c r="A13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
@@ -1017,13 +1023,13 @@
     </row>
     <row r="14" spans="1:26">
       <c r="A14" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
@@ -1051,13 +1057,13 @@
     </row>
     <row r="15" spans="1:26">
       <c r="A15" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="3"/>
       <c r="E15" s="3"/>
@@ -1085,10 +1091,10 @@
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -1117,13 +1123,13 @@
     </row>
     <row r="17" spans="1:26">
       <c r="A17" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
@@ -1151,9 +1157,11 @@
     </row>
     <row r="18" spans="1:26">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
@@ -1181,7 +1189,7 @@
     </row>
     <row r="19" spans="1:26">
       <c r="A19" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1211,10 +1219,10 @@
     </row>
     <row r="20" spans="1:26">
       <c r="A20" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -1243,7 +1251,7 @@
     </row>
     <row r="21" spans="1:26">
       <c r="A21" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1273,10 +1281,10 @@
     </row>
     <row r="22" spans="1:26">
       <c r="A22" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -1305,9 +1313,11 @@
     </row>
     <row r="23" spans="1:26">
       <c r="A23" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
@@ -1335,13 +1345,13 @@
     </row>
     <row r="24" spans="1:26">
       <c r="A24" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1397,7 +1407,7 @@
     </row>
     <row r="26" spans="1:26">
       <c r="A26" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1427,10 +1437,10 @@
     </row>
     <row r="27" spans="1:26">
       <c r="A27" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>53</v>
@@ -1461,10 +1471,10 @@
     </row>
     <row r="28" spans="1:26">
       <c r="A28" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>53</v>
@@ -1495,10 +1505,10 @@
     </row>
     <row r="29" spans="1:26">
       <c r="A29" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>54</v>
@@ -1529,13 +1539,13 @@
     </row>
     <row r="30" spans="1:26">
       <c r="A30" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1563,10 +1573,10 @@
     </row>
     <row r="31" spans="1:26">
       <c r="A31" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>54</v>
@@ -1597,13 +1607,13 @@
     </row>
     <row r="32" spans="1:26">
       <c r="A32" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
@@ -1631,13 +1641,13 @@
     </row>
     <row r="33" spans="1:26">
       <c r="A33" s="6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
@@ -1665,13 +1675,13 @@
     </row>
     <row r="34" spans="1:26">
       <c r="A34" s="6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
@@ -1699,13 +1709,13 @@
     </row>
     <row r="35" spans="1:26">
       <c r="A35" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
@@ -1733,13 +1743,13 @@
     </row>
     <row r="36" spans="1:26">
       <c r="A36" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
@@ -1767,13 +1777,13 @@
     </row>
     <row r="37" spans="1:26">
       <c r="A37" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1829,7 +1839,7 @@
     </row>
     <row r="39" spans="1:26">
       <c r="A39" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -1859,13 +1869,13 @@
     </row>
     <row r="40" spans="1:26">
       <c r="A40" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
@@ -1893,13 +1903,13 @@
     </row>
     <row r="41" spans="1:26">
       <c r="A41" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
@@ -1955,7 +1965,7 @@
     </row>
     <row r="43" spans="1:26">
       <c r="A43" s="4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>

</xml_diff>

<commit_message>
Fixed Camera scene, Added display text
</commit_message>
<xml_diff>
--- a/CG Lab Project Submission Checklist.xlsx
+++ b/CG Lab Project Submission Checklist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fritsch\Google Drive\Personal\Studium\4. Semester\Computer Graphics\cg_lab_2017-master\00_empty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Personal\Studium\4. Semester\Computer Graphics\cg_lab_2017-master\00_empty\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="57">
   <si>
     <t>Project Name:</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Billboarding / Fence / Floor</t>
+  </si>
+  <si>
+    <t>Freecam and Camera Path</t>
   </si>
 </sst>
 </file>
@@ -588,15 +591,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="39.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" customWidth="1"/>
-    <col min="3" max="3" width="66.453125" customWidth="1"/>
+    <col min="1" max="1" width="39.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" customWidth="1"/>
+    <col min="3" max="3" width="66.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -1191,7 +1194,9 @@
       <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="3"/>
@@ -1253,8 +1258,12 @@
       <c r="A21" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>

</xml_diff>